<commit_message>
Feat: finished ED: wk intw portf
</commit_message>
<xml_diff>
--- a/data/ED/program_useful_link.xlsx
+++ b/data/ED/program_useful_link.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB530"/>
+  <dimension ref="A1:AI530"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1098,35 +1098,30 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGCASWMH1F</t>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
+          <t>How to apply:#proxy_collapseHowToApply</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -5901,40 +5896,50 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCCEIDE1F</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCCEIDE1P</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
-        </is>
-      </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
-        </is>
-      </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
       <c r="R62" t="inlineStr">
+        <is>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -10117,40 +10122,125 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDCAP1F</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDCAP1P</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDCAP2P</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDUCD1F</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDUCD1P</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDUCD2P</t>
+        </is>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDURE2F</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDURE3P</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEDURE4P</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEECPF1F</t>
+        </is>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEECPF1P</t>
+        </is>
+      </c>
+      <c r="V110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEECPF2P</t>
+        </is>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEPHOE1F</t>
+        </is>
+      </c>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEPHOE1P</t>
+        </is>
+      </c>
+      <c r="Y110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCEPHOE2P</t>
+        </is>
+      </c>
+      <c r="Z110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGCEECPF1F</t>
+        </is>
+      </c>
+      <c r="AA110" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDEECPF1F</t>
+        </is>
+      </c>
+      <c r="AB110" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
-        </is>
-      </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
-        </is>
-      </c>
-      <c r="N110" t="inlineStr">
-        <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
-        </is>
-      </c>
-      <c r="O110" t="inlineStr">
+      <c r="AC110" t="inlineStr">
+        <is>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
+        </is>
+      </c>
+      <c r="AD110" t="inlineStr">
+        <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="AE110" t="inlineStr">
+        <is>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+        </is>
+      </c>
+      <c r="AF110" t="inlineStr">
         <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="P110" t="inlineStr">
-        <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
-        </is>
-      </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
-      <c r="R110" t="inlineStr">
+      <c r="AG110" t="inlineStr">
+        <is>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+        </is>
+      </c>
+      <c r="AH110" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="AI110" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -18721,40 +18811,70 @@
       </c>
       <c r="K207" t="inlineStr">
         <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCLANIC1U</t>
+        </is>
+      </c>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCLANIC1F</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCLANIC1P</t>
+        </is>
+      </c>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDLANIC1U</t>
+        </is>
+      </c>
+      <c r="O207" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGCLANIC1U</t>
+        </is>
+      </c>
+      <c r="P207" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDLANIC1F</t>
+        </is>
+      </c>
+      <c r="Q207" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="L207" t="inlineStr">
-        <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
-        </is>
-      </c>
-      <c r="M207" t="inlineStr">
-        <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
-        </is>
-      </c>
-      <c r="N207" t="inlineStr">
-        <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
-        </is>
-      </c>
-      <c r="O207" t="inlineStr">
+      <c r="R207" t="inlineStr">
+        <is>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
+        </is>
+      </c>
+      <c r="S207" t="inlineStr">
+        <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="T207" t="inlineStr">
+        <is>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+        </is>
+      </c>
+      <c r="U207" t="inlineStr">
         <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="P207" t="inlineStr">
-        <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
-        </is>
-      </c>
-      <c r="Q207" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
-      <c r="R207" t="inlineStr">
+      <c r="V207" t="inlineStr">
+        <is>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+        </is>
+      </c>
+      <c r="W207" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="X207" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -18810,40 +18930,55 @@
       </c>
       <c r="K208" t="inlineStr">
         <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCLANED1F</t>
+        </is>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCLANED1P</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDLANED1F</t>
+        </is>
+      </c>
+      <c r="N208" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="L208" t="inlineStr">
-        <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
-        </is>
-      </c>
-      <c r="M208" t="inlineStr">
-        <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
-        </is>
-      </c>
-      <c r="N208" t="inlineStr">
-        <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
-        </is>
-      </c>
       <c r="O208" t="inlineStr">
         <is>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
+        </is>
+      </c>
+      <c r="P208" t="inlineStr">
+        <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="Q208" t="inlineStr">
+        <is>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+        </is>
+      </c>
+      <c r="R208" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="P208" t="inlineStr">
-        <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
-        </is>
-      </c>
-      <c r="Q208" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
-      <c r="R208" t="inlineStr">
+      <c r="S208" t="inlineStr">
+        <is>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+        </is>
+      </c>
+      <c r="T208" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="U208" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -27806,40 +27941,65 @@
       </c>
       <c r="K313" t="inlineStr">
         <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCTESOL1U</t>
+        </is>
+      </c>
+      <c r="L313" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTMSCTESOL1F</t>
+        </is>
+      </c>
+      <c r="M313" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDTESOL1U</t>
+        </is>
+      </c>
+      <c r="N313" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGCTESOL1U</t>
+        </is>
+      </c>
+      <c r="O313" t="inlineStr">
+        <is>
+          <t>Tuition fees:http://www.ed.ac.uk/studying/postgraduate/fees?programme_code=PTPGDTESOL1F</t>
+        </is>
+      </c>
+      <c r="P313" t="inlineStr">
+        <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="L313" t="inlineStr">
-        <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
-        </is>
-      </c>
-      <c r="M313" t="inlineStr">
-        <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
-        </is>
-      </c>
-      <c r="N313" t="inlineStr">
-        <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
-        </is>
-      </c>
-      <c r="O313" t="inlineStr">
+      <c r="Q313" t="inlineStr">
+        <is>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
+        </is>
+      </c>
+      <c r="R313" t="inlineStr">
+        <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="S313" t="inlineStr">
+        <is>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
+        </is>
+      </c>
+      <c r="T313" t="inlineStr">
         <is>
           <t>Admissions Office:https://www.ed.ac.uk/arts-humanities-soc-sci/about-us/staff-contacts/college-office</t>
         </is>
       </c>
-      <c r="P313" t="inlineStr">
-        <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
-        </is>
-      </c>
-      <c r="Q313" t="inlineStr">
-        <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
-        </is>
-      </c>
-      <c r="R313" t="inlineStr">
+      <c r="U313" t="inlineStr">
+        <is>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+        </is>
+      </c>
+      <c r="V313" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="W313" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>
@@ -44337,35 +44497,40 @@
       </c>
       <c r="L501" t="inlineStr">
         <is>
-          <t>Application deadlines:#proxy_collapseDeadlines</t>
+          <t>Find out more about the Northern Scholars Scheme PhD scholarship and apply:https://www.ed.ac.uk/student-funding/postgraduate/uk-eu/humanities/literatures-languages-cultures/northern-scholars-scheme-phd-scholarship</t>
         </is>
       </c>
       <c r="M501" t="inlineStr">
         <is>
-          <t>How to apply:#proxy_collapseHowToApply</t>
+          <t>Application deadlines:#proxy_collapseDeadlines</t>
         </is>
       </c>
       <c r="N501" t="inlineStr">
         <is>
+          <t>How to apply:#proxy_collapseHowToApply</t>
+        </is>
+      </c>
+      <c r="O501" t="inlineStr">
+        <is>
           <t>Pre-application guidance:https://www.ed.ac.uk/literatures-languages-cultures/delc/postgraduate/euro-languages-cultures/phd-guidelines</t>
         </is>
       </c>
-      <c r="O501" t="inlineStr">
-        <is>
-          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
-        </is>
-      </c>
       <c r="P501" t="inlineStr">
         <is>
-          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
+          <t>How to apply:http://www.edin.ac/pgdf-apply</t>
         </is>
       </c>
       <c r="Q501" t="inlineStr">
         <is>
-          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+          <t>Privacy statement for applicants:/studying/admissions/privacy-statement</t>
         </is>
       </c>
       <c r="R501" t="inlineStr">
+        <is>
+          <t>Terms and conditions of admission:https://edin.ac/terms</t>
+        </is>
+      </c>
+      <c r="S501" t="inlineStr">
         <is>
           <t>Admissions policies and procedures:/studying/admissions/policies-procedures</t>
         </is>

</xml_diff>